<commit_message>
configured sendgrid, added aggregate query on participants
</commit_message>
<xml_diff>
--- a/participants.xlsx
+++ b/participants.xlsx
@@ -11,14 +11,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>MeetingID</t>
-  </si>
-  <si>
     <t>JoinTime</t>
   </si>
   <si>
@@ -31,19 +28,28 @@
     <t>1RN17CS060 Nithish R</t>
   </si>
   <si>
-    <t>2020-11-17T06:47:53.000Z</t>
-  </si>
-  <si>
-    <t>2020-11-17T06:56:04.000Z</t>
-  </si>
-  <si>
-    <t>Buj</t>
-  </si>
-  <si>
-    <t>2020-11-17T06:54:43.000Z</t>
-  </si>
-  <si>
-    <t>2020-11-17T06:56:20.000Z</t>
+    <t>12:52:08:000+0000</t>
+  </si>
+  <si>
+    <t>14:35:37:000+0000</t>
+  </si>
+  <si>
+    <t>Bujjyo</t>
+  </si>
+  <si>
+    <t>12:54:00:000+0000</t>
+  </si>
+  <si>
+    <t>14:04:18:000+0000</t>
+  </si>
+  <si>
+    <t>1RN17CS067 Pooja.M</t>
+  </si>
+  <si>
+    <t>13:21:49:000+0000</t>
+  </si>
+  <si>
+    <t>14:34:42:000+0000</t>
   </si>
 </sst>
 </file>
@@ -424,13 +430,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="5" width="24" customWidth="1"/>
+    <col min="1" max="4" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,42 +449,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2">
-        <v>74182735820</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>74182735820</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
-        <v>2</v>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>